<commit_message>
partly migrated model in tests/fixtures/migrate/2_species_1_reaction.xlsx
</commit_message>
<xml_diff>
--- a/tests/fixtures/migrate/2_species_1_reaction.xlsx
+++ b/tests/fixtures/migrate/2_species_1_reaction.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_dev_repos/obj_model/tests/fixtures/migrate/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13965" tabRatio="993" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27440" windowHeight="11780" tabRatio="993" firstSheet="7" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -20,32 +25,33 @@
     <sheet name="Reactions" sheetId="10" r:id="rId11"/>
     <sheet name="Rate laws" sheetId="11" r:id="rId12"/>
     <sheet name="dFBA objectives" sheetId="18" r:id="rId13"/>
-    <sheet name="dFBA net reactions" sheetId="12" r:id="rId14"/>
-    <sheet name="dFBA net species" sheetId="13" r:id="rId15"/>
+    <sheet name="dFBA objective reactions" sheetId="12" r:id="rId14"/>
+    <sheet name="dFBA objective species" sheetId="13" r:id="rId15"/>
     <sheet name="Parameters" sheetId="14" r:id="rId16"/>
     <sheet name="Stop conditions" sheetId="15" r:id="rId17"/>
     <sheet name="Evidence" sheetId="19" r:id="rId18"/>
-    <sheet name="References" sheetId="16" r:id="rId19"/>
+    <sheet name="Interpretations" sheetId="22" r:id="rId19"/>
+    <sheet name="References" sheetId="16" r:id="rId20"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Compartments!$A$1:$H$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'dFBA objective reactions'!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'dFBA objective species'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Functions!$A$1:$D$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Initial species concentrations'!$A$1:$E$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Model!$A$1:$B$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Observables!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">Parameters!$A$1:$H$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Rate laws'!$A$1:$G$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Reactions!$A$1:$J$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">References!$A$1:$Q$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Species types'!$A$1:$I$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'Stop conditions'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Submodels!$A$1:$F$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Taxon!$A$1:$A$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Submodels!$A$1:$F$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Compartments!$A$1:$H$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Species types'!$A$1:$I$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Initial species concentrations'!$A$1:$E$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Observables!$A$1:$E$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Functions!$A$1:$D$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Reactions!$A$1:$J$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Rate laws'!$A$1:$G$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'dFBA net reactions'!$A$1:$E$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'dFBA net species'!$A$1:$G$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">Parameters!$A$1:$H$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'Stop conditions'!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">References!$A$1:$Q$1</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="4">Compartments!$A$1:$H$2</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="13">'dFBA net reactions'!$A$1:$E$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="14">'dFBA net species'!$A$1:$G$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="13">'dFBA objective reactions'!$A$1:$E$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="14">'dFBA objective species'!$A$1:$G$1</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="9">Functions!$A$1:$D$1</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="7">'Initial species concentrations'!$A$1:$E$3</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="0">Model!$A$1:$B$8</definedName>
@@ -53,14 +59,14 @@
     <definedName name="_FilterDatabase_0" localSheetId="15">Parameters!$A$1:$H$4</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="11">'Rate laws'!$A$1:$G$2</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="10">Reactions!$A$1:$J$2</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="18">References!$A$1:$Q$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="19">References!$A$1:$Q$1</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="5">'Species types'!$A$1:$I$3</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="16">'Stop conditions'!$A$1:$D$1</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="3">Submodels!$A$1:$F$2</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="1">Taxon!$A$1:$A$5</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="4">Compartments!$A$1:$H$2</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="13">'dFBA net reactions'!$A$1:$E$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="14">'dFBA net species'!$A$1:$G$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="13">'dFBA objective reactions'!$A$1:$E$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="14">'dFBA objective species'!$A$1:$G$1</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="9">Functions!$A$1:$D$1</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="7">'Initial species concentrations'!$A$1:$E$3</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="0">Model!$A$1:$B$8</definedName>
@@ -68,14 +74,14 @@
     <definedName name="_FilterDatabase_0_0" localSheetId="15">Parameters!$A$1:$H$4</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="11">'Rate laws'!$A$1:$G$2</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="10">Reactions!$A$1:$J$2</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="18">References!$A$1:$Q$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="19">References!$A$1:$Q$1</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="5">'Species types'!$A$1:$I$3</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="16">'Stop conditions'!$A$1:$D$1</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="3">Submodels!$A$1:$F$2</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="1">Taxon!$A$1:$A$5</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="4">Compartments!$A$1:$H$2</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="13">'dFBA net reactions'!$A$1:$E$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="14">'dFBA net species'!$A$1:$G$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="13">'dFBA objective reactions'!$A$1:$E$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="14">'dFBA objective species'!$A$1:$G$1</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="9">Functions!$A$1:$D$1</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="7">'Initial species concentrations'!$A$1:$E$3</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="0">Model!$A$1:$B$8</definedName>
@@ -83,18 +89,26 @@
     <definedName name="_FilterDatabase_0_0_0" localSheetId="15">Parameters!$A$1:$H$4</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="11">'Rate laws'!$A$1:$G$2</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="10">Reactions!$A$1:$J$2</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="18">References!$A$1:$Q$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="19">References!$A$1:$Q$1</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="5">'Species types'!$A$1:$I$3</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="16">'Stop conditions'!$A$1:$D$1</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="3">Submodels!$A$1:$F$2</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="1">Taxon!$A$1:$A$5</definedName>
   </definedNames>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="140">
   <si>
     <t>Id</t>
   </si>
@@ -387,9 +401,6 @@
     <t>Cell size units</t>
   </si>
   <si>
-    <t>dFBA net reaction</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -472,19 +483,58 @@
   </si>
   <si>
     <t>Pages</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>interpretation_001</t>
+  </si>
+  <si>
+    <t>Interpretation 001</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>assumption</t>
+  </si>
+  <si>
+    <t>evidence_001_a, evidence_001_b, evidence_001_c</t>
+  </si>
+  <si>
+    <t>interpretation_002</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>approximation</t>
+  </si>
+  <si>
+    <t>evidence_002, evidence_003</t>
+  </si>
+  <si>
+    <t>Interpretations</t>
+  </si>
+  <si>
+    <t>dFBA obj reaction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="28">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -495,197 +545,46 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Menlo"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Cambria"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -710,194 +609,8 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -905,253 +618,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="34" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1180,7 +654,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1204,58 +678,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -1338,10 +769,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="212121"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="F3F3F3"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1585,30 +1016,29 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="19" style="15" customWidth="1"/>
     <col min="2" max="2" width="46.5" style="15" customWidth="1"/>
     <col min="3" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1616,7 +1046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="27" spans="1:2">
+    <row r="2" spans="1:2" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1624,7 +1054,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1632,25 +1062,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="17"/>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="17"/>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -1658,25 +1088,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="18"/>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="18"/>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1684,59 +1114,54 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="19"/>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="19"/>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="19"/>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B15">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <autoFilter ref="A1:B15"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:9">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1756,16 +1181,19 @@
         <v>31</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" customHeight="1" spans="1:9">
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>76</v>
       </c>
@@ -1775,45 +1203,40 @@
       <c r="D2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D2">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <autoFilter ref="A1:D2"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:N2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="L1" sqref="L1:N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.1666666666667" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1"/>
     <col min="3" max="3" width="12.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="29" style="1" customWidth="1"/>
-    <col min="5" max="13" width="9" style="1"/>
-    <col min="14" max="14" width="10" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9" style="1"/>
+    <col min="5" max="14" width="9" style="1"/>
+    <col min="15" max="15" width="10" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:14">
+    <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1848,16 +1271,19 @@
         <v>31</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" s="5" customFormat="1" customHeight="1" spans="1:14">
+    <row r="2" spans="1:15" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>85</v>
       </c>
@@ -1874,47 +1300,42 @@
       <c r="F2" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J2">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <autoFilter ref="A1:J2"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomRight" activeCell="J1" sqref="J1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.66666666666667" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1666666666667" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="4.83333333333333" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.3333333333333" style="1" customWidth="1"/>
-    <col min="7" max="11" width="9" style="1"/>
-    <col min="12" max="12" width="10" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="1"/>
+    <col min="5" max="5" width="4.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="1" customWidth="1"/>
+    <col min="7" max="12" width="9" style="1"/>
+    <col min="13" max="13" width="10" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:12">
+    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1943,16 +1364,19 @@
         <v>31</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" s="5" customFormat="1" customHeight="1" spans="1:12">
+    <row r="2" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>90</v>
       </c>
@@ -1971,41 +1395,36 @@
       <c r="G2" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G2">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <autoFilter ref="A1:G2"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:L1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomRight" activeCell="J1" sqref="J1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="11" width="9" style="1"/>
-    <col min="12" max="12" width="10" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="1"/>
+    <col min="1" max="12" width="9" style="1"/>
+    <col min="13" max="13" width="10" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:12">
+    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2034,40 +1453,40 @@
         <v>31</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:10">
+    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2090,44 +1509,42 @@
         <v>31</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <autoFilter ref="A1:E1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:10">
+    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -2135,13 +1552,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>97</v>
+        <v>139</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>64</v>
@@ -2152,45 +1569,43 @@
       <c r="H1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="2" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <autoFilter ref="A1:G1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:K7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.6666666666667" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" style="1" customWidth="1"/>
     <col min="2" max="5" width="9" style="1"/>
     <col min="6" max="6" width="17.5" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:11">
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2201,10 +1616,10 @@
         <v>57</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>64</v>
@@ -2216,41 +1631,45 @@
         <v>31</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" s="5" customFormat="1" customHeight="1" spans="1:11">
+    <row r="2" spans="1:12" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D2" s="6">
-        <v>6.02214075862e+23</v>
+        <v>6.02214075862E+23</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" s="5" customFormat="1" customHeight="1" spans="1:11">
+    <row r="3" spans="1:12" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>92</v>
@@ -2259,13 +1678,13 @@
         <v>12</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="K3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" s="5" customFormat="1" customHeight="1" spans="1:11">
+    <row r="4" spans="1:12" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>52</v>
       </c>
@@ -2278,19 +1697,20 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="1"/>
+      <c r="L4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" customHeight="1" spans="1:11">
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
@@ -2301,36 +1721,37 @@
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="5"/>
+      <c r="L5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" customHeight="1" spans="1:11">
+    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customHeight="1" spans="1:11">
-      <c r="A7" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
@@ -2341,48 +1762,44 @@
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="5"/>
+      <c r="L7" s="1" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H7">
-    <extLst/>
-  </autoFilter>
+  <autoFilter ref="A1:H7"/>
   <sortState ref="A2:K7">
     <sortCondition ref="A2:A7"/>
   </sortState>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:I1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:9">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2402,44 +1819,42 @@
         <v>31</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <autoFilter ref="A1:D1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:15">
+    <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2447,7 +1862,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>64</v>
@@ -2456,19 +1871,19 @@
         <v>57</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>29</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>16</v>
@@ -2488,29 +1903,230 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3" max="5" width="9" style="1"/>
+    <col min="6" max="6" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7" max="11" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+    </row>
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+    </row>
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+    </row>
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:A7"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:19">
+    <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2518,46 +2134,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>57</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>16</v>
@@ -2570,108 +2186,29 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q1">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="6" outlineLevelCol="1"/>
-  <cols>
-    <col min="1" max="1" width="19" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1666666666667" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" customHeight="1" spans="1:2">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" customHeight="1" spans="1:1">
-      <c r="A2" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" customHeight="1" spans="1:2">
-      <c r="A3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" customHeight="1" spans="1:1">
-      <c r="A4" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" customHeight="1" spans="1:1">
-      <c r="A5" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" customHeight="1" spans="1:1">
-      <c r="A6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" customHeight="1" spans="1:2">
-      <c r="A7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:A7">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <autoFilter ref="A1:Q1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelCol="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:2">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2679,12 +2216,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" customHeight="1" spans="1:1">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" customHeight="1" spans="1:2">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -2692,7 +2229,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" customHeight="1" spans="1:2">
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -2700,7 +2237,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" customHeight="1" spans="1:2">
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>29</v>
       </c>
@@ -2708,22 +2245,22 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="6" customHeight="1" spans="1:1">
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" customHeight="1" spans="1:1">
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" customHeight="1" spans="1:1">
+    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" customHeight="1" spans="1:2">
+    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -2733,37 +2270,34 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="H1" sqref="H1:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" outlineLevelCol="7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83333333333333" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1666666666667" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.8333333333333" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.3333333333333" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6666666666667" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:8">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2789,7 +2323,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" s="5" customFormat="1" customHeight="1" spans="1:8">
+    <row r="2" spans="1:8" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
@@ -2801,34 +2335,29 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F2">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <autoFilter ref="A1:F2"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:Q2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomRight" activeCell="O1" sqref="O1:Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:17">
+    <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -2872,16 +2401,19 @@
         <v>31</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="P1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" s="5" customFormat="1" customHeight="1" spans="1:17">
+    <row r="2" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>44</v>
       </c>
@@ -2905,10 +2437,10 @@
         <v>50</v>
       </c>
       <c r="I2" s="6">
-        <v>4.58e-17</v>
+        <v>4.58E-17</v>
       </c>
       <c r="J2" s="1">
-        <v>4.58e-18</v>
+        <v>4.5800000000000003E-18</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>51</v>
@@ -2916,42 +2448,37 @@
       <c r="L2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H2">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <autoFilter ref="A1:H2"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L3" sqref="L2:L3"/>
+      <selection pane="bottomRight" activeCell="J1" sqref="J1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5" style="1" customWidth="1"/>
-    <col min="2" max="11" width="9" style="1"/>
-    <col min="12" max="12" width="10" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="1"/>
+    <col min="2" max="12" width="9" style="1"/>
+    <col min="13" max="13" width="10" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:12">
+    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2980,16 +2507,19 @@
         <v>31</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" s="5" customFormat="1" customHeight="1" spans="1:12">
+    <row r="2" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>58</v>
       </c>
@@ -3005,11 +2535,11 @@
       <c r="G2" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" s="5" customFormat="1" customHeight="1" spans="1:12">
+    <row r="3" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>61</v>
       </c>
@@ -3025,39 +2555,34 @@
       <c r="G3" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I3">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <autoFilter ref="A1:I3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:J3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J3" sqref="J2:J3"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:10">
+    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3080,16 +2605,19 @@
         <v>31</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" customHeight="1" spans="1:10">
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>65</v>
       </c>
@@ -3102,11 +2630,11 @@
       <c r="E2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" customHeight="1" spans="1:10">
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>67</v>
       </c>
@@ -3119,13 +2647,13 @@
       <c r="E3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3134,27 +2662,25 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomRight" activeCell="J1" sqref="J1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.1666666666667" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1"/>
-    <col min="3" max="3" width="13.1666666666667" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:12">
+    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3183,16 +2709,19 @@
         <v>31</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" customHeight="1" spans="1:12">
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>72</v>
       </c>
@@ -3203,16 +2732,16 @@
         <v>50</v>
       </c>
       <c r="E2" s="1">
-        <v>33.2107808085433</v>
+        <v>33.210780808543298</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" customHeight="1" spans="1:12">
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>74</v>
       </c>
@@ -3228,39 +2757,34 @@
       <c r="G3" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E3">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <autoFilter ref="A1:E3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:I1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:9">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3279,22 +2803,22 @@
       <c r="F1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <autoFilter ref="A1:E1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>